<commit_message>
url id encryption done
</commit_message>
<xml_diff>
--- a/documentation/ProjectDocumentation-Sai.xlsx
+++ b/documentation/ProjectDocumentation-Sai.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\freelancing-projects\WheelPact\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WheelPact_CI4\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77733DD-B58B-4E86-A3EE-CEFC2F0983B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Project Overview" sheetId="1" r:id="rId1"/>
@@ -19,11 +18,12 @@
     <sheet name="Resources" sheetId="5" r:id="rId4"/>
     <sheet name="Module List" sheetId="6" r:id="rId5"/>
     <sheet name="Database Schema" sheetId="7" r:id="rId6"/>
+    <sheet name="Tech Stack" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="2">GanttChart!$A1048576</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,13 +44,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Vertex42</author>
     <author>Vertex42.com Templates</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{3F9B9398-7E95-491D-A8FD-16B4649258CF}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{341902A4-C57D-45A5-97E5-030D316A91C4}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{A2803F5F-BE73-462A-894F-6DD177814995}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{D1FA9A27-BA97-406E-AFB0-DDF86884EE30}">
+    <comment ref="D7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{87C4A890-54E4-4914-A137-F591D668A1CF}">
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="1" shapeId="0" xr:uid="{230BDD35-1397-40B0-A9D8-0D4EAEE09315}">
+    <comment ref="F7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -296,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{4CB8891E-5B82-4D6E-B044-42B637CC1A2C}">
+    <comment ref="G7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -378,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{B1F114E7-F12C-48E7-BCBC-C56E24D3D7BC}">
+    <comment ref="H7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -402,7 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{8A01252C-4F86-49BF-9C89-6987A5812082}">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -431,7 +431,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="159">
   <si>
     <t>brief description of the project</t>
   </si>
@@ -884,12 +884,36 @@
   </si>
   <si>
     <t>Mobile App</t>
+  </si>
+  <si>
+    <t>Front End</t>
+  </si>
+  <si>
+    <t>Back End</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Hosting</t>
+  </si>
+  <si>
+    <t>PHP- Codeigniter 4</t>
+  </si>
+  <si>
+    <t>HTML,CSS,Bootstrap 4,Jquery</t>
+  </si>
+  <si>
+    <t>MySql</t>
+  </si>
+  <si>
+    <t>Hostinger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ \(dddd\)"/>
     <numFmt numFmtId="165" formatCode="d\ mmm\ yyyy"/>
@@ -1458,14 +1482,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1476,23 +1500,23 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1561,15 +1585,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>99060</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>160020</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1871,39 +1895,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1914,42 +1938,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6E4B55-C2DF-4E80-8ED8-A5C7E3BCE197}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C56368-5B03-42B0-B8A1-7B3ED68525F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" customWidth="1"/>
-    <col min="10" max="10" width="1.88671875" customWidth="1"/>
-    <col min="11" max="108" width="2.44140625" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" customWidth="1"/>
+    <col min="10" max="10" width="1.85546875" customWidth="1"/>
+    <col min="11" max="108" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:108" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -1959,29 +1983,29 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="I1" s="3"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-    </row>
-    <row r="2" spans="1:108" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+    </row>
+    <row r="2" spans="1:108" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
@@ -1992,7 +2016,7 @@
       <c r="F2" s="7"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="9"/>
       <c r="H3" s="8"/>
@@ -2014,16 +2038,16 @@
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:108" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:108" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="68">
+      <c r="C4" s="69">
         <v>45082</v>
       </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11"/>
       <c r="G4" s="12" t="s">
         <v>6</v>
@@ -2033,304 +2057,304 @@
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="14"/>
-      <c r="K4" s="63" t="str">
+      <c r="K4" s="65" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="63" t="str">
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="65" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="65"/>
-      <c r="Y4" s="63" t="str">
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="65" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="64"/>
-      <c r="AA4" s="64"/>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="64"/>
-      <c r="AD4" s="64"/>
-      <c r="AE4" s="65"/>
-      <c r="AF4" s="63" t="str">
+      <c r="Z4" s="66"/>
+      <c r="AA4" s="66"/>
+      <c r="AB4" s="66"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="67"/>
+      <c r="AF4" s="65" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="64"/>
-      <c r="AH4" s="64"/>
-      <c r="AI4" s="64"/>
-      <c r="AJ4" s="64"/>
-      <c r="AK4" s="64"/>
-      <c r="AL4" s="65"/>
-      <c r="AM4" s="63" t="str">
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="66"/>
+      <c r="AI4" s="66"/>
+      <c r="AJ4" s="66"/>
+      <c r="AK4" s="66"/>
+      <c r="AL4" s="67"/>
+      <c r="AM4" s="65" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="64"/>
-      <c r="AO4" s="64"/>
-      <c r="AP4" s="64"/>
-      <c r="AQ4" s="64"/>
-      <c r="AR4" s="64"/>
-      <c r="AS4" s="65"/>
-      <c r="AT4" s="63" t="str">
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="66"/>
+      <c r="AQ4" s="66"/>
+      <c r="AR4" s="66"/>
+      <c r="AS4" s="67"/>
+      <c r="AT4" s="65" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="64"/>
-      <c r="AV4" s="64"/>
-      <c r="AW4" s="64"/>
-      <c r="AX4" s="64"/>
-      <c r="AY4" s="64"/>
-      <c r="AZ4" s="65"/>
-      <c r="BA4" s="63" t="str">
+      <c r="AU4" s="66"/>
+      <c r="AV4" s="66"/>
+      <c r="AW4" s="66"/>
+      <c r="AX4" s="66"/>
+      <c r="AY4" s="66"/>
+      <c r="AZ4" s="67"/>
+      <c r="BA4" s="65" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="64"/>
-      <c r="BC4" s="64"/>
-      <c r="BD4" s="64"/>
-      <c r="BE4" s="64"/>
-      <c r="BF4" s="64"/>
-      <c r="BG4" s="65"/>
-      <c r="BH4" s="63" t="str">
+      <c r="BB4" s="66"/>
+      <c r="BC4" s="66"/>
+      <c r="BD4" s="66"/>
+      <c r="BE4" s="66"/>
+      <c r="BF4" s="66"/>
+      <c r="BG4" s="67"/>
+      <c r="BH4" s="65" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="64"/>
-      <c r="BJ4" s="64"/>
-      <c r="BK4" s="64"/>
-      <c r="BL4" s="64"/>
-      <c r="BM4" s="64"/>
-      <c r="BN4" s="65"/>
-      <c r="BO4" s="63" t="str">
+      <c r="BI4" s="66"/>
+      <c r="BJ4" s="66"/>
+      <c r="BK4" s="66"/>
+      <c r="BL4" s="66"/>
+      <c r="BM4" s="66"/>
+      <c r="BN4" s="67"/>
+      <c r="BO4" s="65" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BP4" s="64"/>
-      <c r="BQ4" s="64"/>
-      <c r="BR4" s="64"/>
-      <c r="BS4" s="64"/>
-      <c r="BT4" s="64"/>
-      <c r="BU4" s="65"/>
-      <c r="BV4" s="63" t="str">
+      <c r="BP4" s="66"/>
+      <c r="BQ4" s="66"/>
+      <c r="BR4" s="66"/>
+      <c r="BS4" s="66"/>
+      <c r="BT4" s="66"/>
+      <c r="BU4" s="67"/>
+      <c r="BV4" s="65" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BW4" s="64"/>
-      <c r="BX4" s="64"/>
-      <c r="BY4" s="64"/>
-      <c r="BZ4" s="64"/>
-      <c r="CA4" s="64"/>
-      <c r="CB4" s="65"/>
-      <c r="CC4" s="63" t="str">
+      <c r="BW4" s="66"/>
+      <c r="BX4" s="66"/>
+      <c r="BY4" s="66"/>
+      <c r="BZ4" s="66"/>
+      <c r="CA4" s="66"/>
+      <c r="CB4" s="67"/>
+      <c r="CC4" s="65" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CD4" s="64"/>
-      <c r="CE4" s="64"/>
-      <c r="CF4" s="64"/>
-      <c r="CG4" s="64"/>
-      <c r="CH4" s="64"/>
-      <c r="CI4" s="65"/>
-      <c r="CJ4" s="63" t="str">
+      <c r="CD4" s="66"/>
+      <c r="CE4" s="66"/>
+      <c r="CF4" s="66"/>
+      <c r="CG4" s="66"/>
+      <c r="CH4" s="66"/>
+      <c r="CI4" s="67"/>
+      <c r="CJ4" s="65" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CK4" s="64"/>
-      <c r="CL4" s="64"/>
-      <c r="CM4" s="64"/>
-      <c r="CN4" s="64"/>
-      <c r="CO4" s="64"/>
-      <c r="CP4" s="65"/>
-      <c r="CQ4" s="63" t="str">
+      <c r="CK4" s="66"/>
+      <c r="CL4" s="66"/>
+      <c r="CM4" s="66"/>
+      <c r="CN4" s="66"/>
+      <c r="CO4" s="66"/>
+      <c r="CP4" s="67"/>
+      <c r="CQ4" s="65" t="str">
         <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="CR4" s="64"/>
-      <c r="CS4" s="64"/>
-      <c r="CT4" s="64"/>
-      <c r="CU4" s="64"/>
-      <c r="CV4" s="64"/>
-      <c r="CW4" s="65"/>
-      <c r="CX4" s="63" t="str">
+      <c r="CR4" s="66"/>
+      <c r="CS4" s="66"/>
+      <c r="CT4" s="66"/>
+      <c r="CU4" s="66"/>
+      <c r="CV4" s="66"/>
+      <c r="CW4" s="67"/>
+      <c r="CX4" s="65" t="str">
         <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="CY4" s="64"/>
-      <c r="CZ4" s="64"/>
-      <c r="DA4" s="64"/>
-      <c r="DB4" s="64"/>
-      <c r="DC4" s="64"/>
-      <c r="DD4" s="65"/>
-    </row>
-    <row r="5" spans="1:108" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="CY4" s="66"/>
+      <c r="CZ4" s="66"/>
+      <c r="DA4" s="66"/>
+      <c r="DB4" s="66"/>
+      <c r="DC4" s="66"/>
+      <c r="DD4" s="67"/>
+    </row>
+    <row r="5" spans="1:108" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="60">
+      <c r="K5" s="71">
         <f>K6</f>
         <v>45082</v>
       </c>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="60">
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="71">
         <f>R6</f>
         <v>45089</v>
       </c>
-      <c r="S5" s="61"/>
-      <c r="T5" s="61"/>
-      <c r="U5" s="61"/>
-      <c r="V5" s="61"/>
-      <c r="W5" s="61"/>
-      <c r="X5" s="62"/>
-      <c r="Y5" s="60">
+      <c r="S5" s="72"/>
+      <c r="T5" s="72"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="73"/>
+      <c r="Y5" s="71">
         <f>Y6</f>
         <v>45096</v>
       </c>
-      <c r="Z5" s="61"/>
-      <c r="AA5" s="61"/>
-      <c r="AB5" s="61"/>
-      <c r="AC5" s="61"/>
-      <c r="AD5" s="61"/>
-      <c r="AE5" s="62"/>
-      <c r="AF5" s="60">
+      <c r="Z5" s="72"/>
+      <c r="AA5" s="72"/>
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="72"/>
+      <c r="AE5" s="73"/>
+      <c r="AF5" s="71">
         <f>AF6</f>
         <v>45103</v>
       </c>
-      <c r="AG5" s="61"/>
-      <c r="AH5" s="61"/>
-      <c r="AI5" s="61"/>
-      <c r="AJ5" s="61"/>
-      <c r="AK5" s="61"/>
-      <c r="AL5" s="62"/>
-      <c r="AM5" s="60">
+      <c r="AG5" s="72"/>
+      <c r="AH5" s="72"/>
+      <c r="AI5" s="72"/>
+      <c r="AJ5" s="72"/>
+      <c r="AK5" s="72"/>
+      <c r="AL5" s="73"/>
+      <c r="AM5" s="71">
         <f>AM6</f>
         <v>45110</v>
       </c>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="61"/>
-      <c r="AP5" s="61"/>
-      <c r="AQ5" s="61"/>
-      <c r="AR5" s="61"/>
-      <c r="AS5" s="62"/>
-      <c r="AT5" s="60">
+      <c r="AN5" s="72"/>
+      <c r="AO5" s="72"/>
+      <c r="AP5" s="72"/>
+      <c r="AQ5" s="72"/>
+      <c r="AR5" s="72"/>
+      <c r="AS5" s="73"/>
+      <c r="AT5" s="71">
         <f>AT6</f>
         <v>45117</v>
       </c>
-      <c r="AU5" s="61"/>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="61"/>
-      <c r="AX5" s="61"/>
-      <c r="AY5" s="61"/>
-      <c r="AZ5" s="62"/>
-      <c r="BA5" s="60">
+      <c r="AU5" s="72"/>
+      <c r="AV5" s="72"/>
+      <c r="AW5" s="72"/>
+      <c r="AX5" s="72"/>
+      <c r="AY5" s="72"/>
+      <c r="AZ5" s="73"/>
+      <c r="BA5" s="71">
         <f>BA6</f>
         <v>45124</v>
       </c>
-      <c r="BB5" s="61"/>
-      <c r="BC5" s="61"/>
-      <c r="BD5" s="61"/>
-      <c r="BE5" s="61"/>
-      <c r="BF5" s="61"/>
-      <c r="BG5" s="62"/>
-      <c r="BH5" s="60">
+      <c r="BB5" s="72"/>
+      <c r="BC5" s="72"/>
+      <c r="BD5" s="72"/>
+      <c r="BE5" s="72"/>
+      <c r="BF5" s="72"/>
+      <c r="BG5" s="73"/>
+      <c r="BH5" s="71">
         <f>BH6</f>
         <v>45131</v>
       </c>
-      <c r="BI5" s="61"/>
-      <c r="BJ5" s="61"/>
-      <c r="BK5" s="61"/>
-      <c r="BL5" s="61"/>
-      <c r="BM5" s="61"/>
-      <c r="BN5" s="62"/>
-      <c r="BO5" s="60">
+      <c r="BI5" s="72"/>
+      <c r="BJ5" s="72"/>
+      <c r="BK5" s="72"/>
+      <c r="BL5" s="72"/>
+      <c r="BM5" s="72"/>
+      <c r="BN5" s="73"/>
+      <c r="BO5" s="71">
         <f>BO6</f>
         <v>45138</v>
       </c>
-      <c r="BP5" s="61"/>
-      <c r="BQ5" s="61"/>
-      <c r="BR5" s="61"/>
-      <c r="BS5" s="61"/>
-      <c r="BT5" s="61"/>
-      <c r="BU5" s="62"/>
-      <c r="BV5" s="60">
+      <c r="BP5" s="72"/>
+      <c r="BQ5" s="72"/>
+      <c r="BR5" s="72"/>
+      <c r="BS5" s="72"/>
+      <c r="BT5" s="72"/>
+      <c r="BU5" s="73"/>
+      <c r="BV5" s="71">
         <f>BV6</f>
         <v>45145</v>
       </c>
-      <c r="BW5" s="61"/>
-      <c r="BX5" s="61"/>
-      <c r="BY5" s="61"/>
-      <c r="BZ5" s="61"/>
-      <c r="CA5" s="61"/>
-      <c r="CB5" s="62"/>
-      <c r="CC5" s="60">
+      <c r="BW5" s="72"/>
+      <c r="BX5" s="72"/>
+      <c r="BY5" s="72"/>
+      <c r="BZ5" s="72"/>
+      <c r="CA5" s="72"/>
+      <c r="CB5" s="73"/>
+      <c r="CC5" s="71">
         <f>CC6</f>
         <v>45152</v>
       </c>
-      <c r="CD5" s="61"/>
-      <c r="CE5" s="61"/>
-      <c r="CF5" s="61"/>
-      <c r="CG5" s="61"/>
-      <c r="CH5" s="61"/>
-      <c r="CI5" s="62"/>
-      <c r="CJ5" s="60">
+      <c r="CD5" s="72"/>
+      <c r="CE5" s="72"/>
+      <c r="CF5" s="72"/>
+      <c r="CG5" s="72"/>
+      <c r="CH5" s="72"/>
+      <c r="CI5" s="73"/>
+      <c r="CJ5" s="71">
         <f>CJ6</f>
         <v>45159</v>
       </c>
-      <c r="CK5" s="61"/>
-      <c r="CL5" s="61"/>
-      <c r="CM5" s="61"/>
-      <c r="CN5" s="61"/>
-      <c r="CO5" s="61"/>
-      <c r="CP5" s="62"/>
-      <c r="CQ5" s="60">
+      <c r="CK5" s="72"/>
+      <c r="CL5" s="72"/>
+      <c r="CM5" s="72"/>
+      <c r="CN5" s="72"/>
+      <c r="CO5" s="72"/>
+      <c r="CP5" s="73"/>
+      <c r="CQ5" s="71">
         <f>CQ6</f>
         <v>45166</v>
       </c>
-      <c r="CR5" s="61"/>
-      <c r="CS5" s="61"/>
-      <c r="CT5" s="61"/>
-      <c r="CU5" s="61"/>
-      <c r="CV5" s="61"/>
-      <c r="CW5" s="62"/>
-      <c r="CX5" s="60">
+      <c r="CR5" s="72"/>
+      <c r="CS5" s="72"/>
+      <c r="CT5" s="72"/>
+      <c r="CU5" s="72"/>
+      <c r="CV5" s="72"/>
+      <c r="CW5" s="73"/>
+      <c r="CX5" s="71">
         <f>CX6</f>
         <v>45173</v>
       </c>
-      <c r="CY5" s="61"/>
-      <c r="CZ5" s="61"/>
-      <c r="DA5" s="61"/>
-      <c r="DB5" s="61"/>
-      <c r="DC5" s="61"/>
-      <c r="DD5" s="62"/>
-    </row>
-    <row r="6" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="CY5" s="72"/>
+      <c r="CZ5" s="72"/>
+      <c r="DA5" s="72"/>
+      <c r="DB5" s="72"/>
+      <c r="DC5" s="72"/>
+      <c r="DD5" s="73"/>
+    </row>
+    <row r="6" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -2734,7 +2758,7 @@
         <v>45179</v>
       </c>
     </row>
-    <row r="7" spans="1:108" s="9" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:108" s="9" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>9</v>
       </c>
@@ -3156,7 +3180,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="8" spans="1:108" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:108" s="36" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -3168,13 +3192,13 @@
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
       <c r="F8" s="30" t="str">
-        <f>IF(ISBLANK(E8)," - ",IF(G8=0,E8,E8+G8-1))</f>
+        <f t="shared" ref="F8:F13" si="4">IF(ISBLANK(E8)," - ",IF(G8=0,E8,E8+G8-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G8" s="31"/>
       <c r="H8" s="32"/>
       <c r="I8" s="33" t="str">
-        <f t="shared" ref="I8:I54" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I54" si="5">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="34"/>
@@ -3277,9 +3301,9 @@
       <c r="DC8" s="35"/>
       <c r="DD8" s="35"/>
     </row>
-    <row r="9" spans="1:108" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:108" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="str">
-        <f t="shared" ref="A9:A10" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A9:A10" si="6">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B9" s="38" t="s">
@@ -3290,7 +3314,7 @@
         <v>45083</v>
       </c>
       <c r="F9" s="42">
-        <f>IF(ISBLANK(E9)," - ",IF(G9=0,E9,E9+G9-1))</f>
+        <f t="shared" si="4"/>
         <v>45085</v>
       </c>
       <c r="G9" s="43">
@@ -3403,9 +3427,9 @@
       <c r="DC9" s="37"/>
       <c r="DD9" s="37"/>
     </row>
-    <row r="10" spans="1:108" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:108" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.2</v>
       </c>
       <c r="B10" s="38" t="s">
@@ -3416,7 +3440,7 @@
         <v>45086</v>
       </c>
       <c r="F10" s="42">
-        <f>IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+        <f t="shared" si="4"/>
         <v>45088</v>
       </c>
       <c r="G10" s="43">
@@ -3529,9 +3553,9 @@
       <c r="DC10" s="37"/>
       <c r="DD10" s="37"/>
     </row>
-    <row r="11" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="str">
-        <f t="shared" ref="A11" si="6">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A11" si="7">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.3</v>
       </c>
       <c r="B11" s="38" t="s">
@@ -3542,7 +3566,7 @@
         <v>45089</v>
       </c>
       <c r="F11" s="42">
-        <f>IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+        <f t="shared" si="4"/>
         <v>45103</v>
       </c>
       <c r="G11" s="43">
@@ -3655,7 +3679,7 @@
       <c r="DC11" s="37"/>
       <c r="DD11" s="37"/>
     </row>
-    <row r="12" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.1</v>
@@ -3668,7 +3692,7 @@
         <v>45075</v>
       </c>
       <c r="F12" s="42">
-        <f>IF(ISBLANK(E12)," - ",IF(G12=0,E12,E12+G12-1))</f>
+        <f t="shared" si="4"/>
         <v>45079</v>
       </c>
       <c r="G12" s="43">
@@ -3781,7 +3805,7 @@
       <c r="DC12" s="37"/>
       <c r="DD12" s="37"/>
     </row>
-    <row r="13" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.2</v>
@@ -3794,7 +3818,7 @@
         <v>45075</v>
       </c>
       <c r="F13" s="42">
-        <f>IF(ISBLANK(E13)," - ",IF(G13=0,E13,E13+G13-1))</f>
+        <f t="shared" si="4"/>
         <v>45076</v>
       </c>
       <c r="G13" s="43">
@@ -3907,9 +3931,9 @@
       <c r="DC13" s="37"/>
       <c r="DD13" s="37"/>
     </row>
-    <row r="14" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="str">
-        <f t="shared" ref="A14" si="7">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A14" si="8">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.4</v>
       </c>
       <c r="B14" s="38" t="s">
@@ -3920,7 +3944,7 @@
         <v>45084</v>
       </c>
       <c r="F14" s="42">
-        <f t="shared" ref="F14:F16" si="8">IF(ISBLANK(E14)," - ",IF(G14=0,E14,E14+G14-1))</f>
+        <f t="shared" ref="F14:F16" si="9">IF(ISBLANK(E14)," - ",IF(G14=0,E14,E14+G14-1))</f>
         <v>45086</v>
       </c>
       <c r="G14" s="43">
@@ -3930,7 +3954,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="45">
-        <f t="shared" ref="I14:I16" si="9">IF(OR(F14=0,E14=0)," - ",NETWORKDAYS(E14,F14))</f>
+        <f t="shared" ref="I14:I16" si="10">IF(OR(F14=0,E14=0)," - ",NETWORKDAYS(E14,F14))</f>
         <v>3</v>
       </c>
       <c r="J14" s="46"/>
@@ -4033,9 +4057,9 @@
       <c r="DC14" s="37"/>
       <c r="DD14" s="37"/>
     </row>
-    <row r="15" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="str">
-        <f t="shared" ref="A15:A16" si="10">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" ref="A15:A16" si="11">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.4.1</v>
       </c>
       <c r="B15" s="47" t="s">
@@ -4046,7 +4070,7 @@
         <v>45084</v>
       </c>
       <c r="F15" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>45084</v>
       </c>
       <c r="G15" s="43">
@@ -4056,7 +4080,7 @@
         <v>0.05</v>
       </c>
       <c r="I15" s="45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J15" s="46"/>
@@ -4159,9 +4183,9 @@
       <c r="DC15" s="37"/>
       <c r="DD15" s="37"/>
     </row>
-    <row r="16" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.4.2</v>
       </c>
       <c r="B16" s="47" t="s">
@@ -4172,7 +4196,7 @@
         <v>45084</v>
       </c>
       <c r="F16" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>45084</v>
       </c>
       <c r="G16" s="43">
@@ -4182,7 +4206,7 @@
         <v>0.05</v>
       </c>
       <c r="I16" s="45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J16" s="46"/>
@@ -4285,9 +4309,9 @@
       <c r="DC16" s="37"/>
       <c r="DD16" s="37"/>
     </row>
-    <row r="17" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="str">
-        <f t="shared" ref="A17:A19" si="11">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A17:A19" si="12">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.5</v>
       </c>
       <c r="B17" s="38" t="s">
@@ -4298,7 +4322,7 @@
         <v>45082</v>
       </c>
       <c r="F17" s="42">
-        <f t="shared" ref="F17:F54" si="12">IF(ISBLANK(E17)," - ",IF(G17=0,E17,E17+G17-1))</f>
+        <f t="shared" ref="F17:F54" si="13">IF(ISBLANK(E17)," - ",IF(G17=0,E17,E17+G17-1))</f>
         <v>45083</v>
       </c>
       <c r="G17" s="43">
@@ -4308,7 +4332,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J17" s="46"/>
@@ -4411,7 +4435,7 @@
       <c r="DC17" s="37"/>
       <c r="DD17" s="37"/>
     </row>
-    <row r="18" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.5.1</v>
@@ -4424,7 +4448,7 @@
         <v>45082</v>
       </c>
       <c r="F18" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45082</v>
       </c>
       <c r="G18" s="43">
@@ -4434,7 +4458,7 @@
         <v>0.05</v>
       </c>
       <c r="I18" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J18" s="46"/>
@@ -4537,9 +4561,9 @@
       <c r="DC18" s="37"/>
       <c r="DD18" s="37"/>
     </row>
-    <row r="19" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6</v>
       </c>
       <c r="B19" s="38" t="s">
@@ -4550,7 +4574,7 @@
         <v>45084</v>
       </c>
       <c r="F19" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45086</v>
       </c>
       <c r="G19" s="43">
@@ -4560,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J19" s="46"/>
@@ -4663,7 +4687,7 @@
       <c r="DC19" s="37"/>
       <c r="DD19" s="37"/>
     </row>
-    <row r="20" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.6.1</v>
@@ -4676,7 +4700,7 @@
         <v>45084</v>
       </c>
       <c r="F20" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45084</v>
       </c>
       <c r="G20" s="43">
@@ -4686,7 +4710,7 @@
         <v>0.05</v>
       </c>
       <c r="I20" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J20" s="46"/>
@@ -4789,9 +4813,9 @@
       <c r="DC20" s="37"/>
       <c r="DD20" s="37"/>
     </row>
-    <row r="21" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="str">
-        <f t="shared" ref="A21" si="13">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A21" si="14">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.7</v>
       </c>
       <c r="B21" s="38" t="s">
@@ -4802,7 +4826,7 @@
         <v>45084</v>
       </c>
       <c r="F21" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45086</v>
       </c>
       <c r="G21" s="43">
@@ -4812,7 +4836,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J21" s="46"/>
@@ -4915,7 +4939,7 @@
       <c r="DC21" s="37"/>
       <c r="DD21" s="37"/>
     </row>
-    <row r="22" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.7.1</v>
@@ -4928,7 +4952,7 @@
         <v>45084</v>
       </c>
       <c r="F22" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45084</v>
       </c>
       <c r="G22" s="43">
@@ -4938,7 +4962,7 @@
         <v>0.05</v>
       </c>
       <c r="I22" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J22" s="46"/>
@@ -5041,7 +5065,7 @@
       <c r="DC22" s="37"/>
       <c r="DD22" s="37"/>
     </row>
-    <row r="23" spans="1:108" s="36" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:108" s="36" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -5052,13 +5076,13 @@
       <c r="D23" s="50"/>
       <c r="E23" s="51"/>
       <c r="F23" s="51" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G23" s="52"/>
       <c r="H23" s="53"/>
       <c r="I23" s="54" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J23" s="55"/>
@@ -5161,9 +5185,9 @@
       <c r="DC23" s="56"/>
       <c r="DD23" s="56"/>
     </row>
-    <row r="24" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:108" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="str">
-        <f t="shared" ref="A24:A26" si="14">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A24:A26" si="15">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B24" s="38" t="s">
@@ -5174,7 +5198,7 @@
         <v>45084</v>
       </c>
       <c r="F24" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45086</v>
       </c>
       <c r="G24" s="43">
@@ -5184,7 +5208,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J24" s="46"/>
@@ -5287,9 +5311,9 @@
       <c r="DC24" s="37"/>
       <c r="DD24" s="37"/>
     </row>
-    <row r="25" spans="1:108" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:108" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.2</v>
       </c>
       <c r="B25" s="38" t="s">
@@ -5300,7 +5324,7 @@
         <v>45084</v>
       </c>
       <c r="F25" s="42">
-        <f t="shared" ref="F25" si="15">IF(ISBLANK(E25)," - ",IF(G25=0,E25,E25+G25-1))</f>
+        <f t="shared" ref="F25" si="16">IF(ISBLANK(E25)," - ",IF(G25=0,E25,E25+G25-1))</f>
         <v>45086</v>
       </c>
       <c r="G25" s="43">
@@ -5310,7 +5334,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="45">
-        <f t="shared" ref="I25" si="16">IF(OR(F25=0,E25=0)," - ",NETWORKDAYS(E25,F25))</f>
+        <f t="shared" ref="I25" si="17">IF(OR(F25=0,E25=0)," - ",NETWORKDAYS(E25,F25))</f>
         <v>3</v>
       </c>
       <c r="J25" s="46"/>
@@ -5413,9 +5437,9 @@
       <c r="DC25" s="37"/>
       <c r="DD25" s="37"/>
     </row>
-    <row r="26" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.3</v>
       </c>
       <c r="B26" s="38" t="s">
@@ -5426,7 +5450,7 @@
         <v>45084</v>
       </c>
       <c r="F26" s="42">
-        <f t="shared" ref="F26" si="17">IF(ISBLANK(E26)," - ",IF(G26=0,E26,E26+G26-1))</f>
+        <f t="shared" ref="F26" si="18">IF(ISBLANK(E26)," - ",IF(G26=0,E26,E26+G26-1))</f>
         <v>45086</v>
       </c>
       <c r="G26" s="43">
@@ -5436,7 +5460,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="45">
-        <f t="shared" ref="I26" si="18">IF(OR(F26=0,E26=0)," - ",NETWORKDAYS(E26,F26))</f>
+        <f t="shared" ref="I26" si="19">IF(OR(F26=0,E26=0)," - ",NETWORKDAYS(E26,F26))</f>
         <v>3</v>
       </c>
       <c r="J26" s="46"/>
@@ -5539,9 +5563,9 @@
       <c r="DC26" s="37"/>
       <c r="DD26" s="37"/>
     </row>
-    <row r="27" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="str">
-        <f t="shared" ref="A27:A39" si="19">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" ref="A27:A39" si="20">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.3.1</v>
       </c>
       <c r="B27" s="47" t="s">
@@ -5552,7 +5576,7 @@
         <v>45084</v>
       </c>
       <c r="F27" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45084</v>
       </c>
       <c r="G27" s="43">
@@ -5562,7 +5586,7 @@
         <v>0.05</v>
       </c>
       <c r="I27" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J27" s="46"/>
@@ -5665,9 +5689,9 @@
       <c r="DC27" s="37"/>
       <c r="DD27" s="37"/>
     </row>
-    <row r="28" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.3.2</v>
       </c>
       <c r="B28" s="47" t="s">
@@ -5678,7 +5702,7 @@
         <v>45084</v>
       </c>
       <c r="F28" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45084</v>
       </c>
       <c r="G28" s="43">
@@ -5688,7 +5712,7 @@
         <v>0.05</v>
       </c>
       <c r="I28" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J28" s="46"/>
@@ -5791,9 +5815,9 @@
       <c r="DC28" s="37"/>
       <c r="DD28" s="37"/>
     </row>
-    <row r="29" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="str">
-        <f t="shared" ref="A29:A37" si="20">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A29:A37" si="21">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.4</v>
       </c>
       <c r="B29" s="38" t="s">
@@ -5804,7 +5828,7 @@
         <v>45084</v>
       </c>
       <c r="F29" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45086</v>
       </c>
       <c r="G29" s="43">
@@ -5814,7 +5838,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J29" s="46"/>
@@ -5917,9 +5941,9 @@
       <c r="DC29" s="37"/>
       <c r="DD29" s="37"/>
     </row>
-    <row r="30" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.4.1</v>
       </c>
       <c r="B30" s="47" t="s">
@@ -5930,7 +5954,7 @@
         <v>45084</v>
       </c>
       <c r="F30" s="42">
-        <f t="shared" ref="F30:F31" si="21">IF(ISBLANK(E30)," - ",IF(G30=0,E30,E30+G30-1))</f>
+        <f t="shared" ref="F30:F31" si="22">IF(ISBLANK(E30)," - ",IF(G30=0,E30,E30+G30-1))</f>
         <v>45084</v>
       </c>
       <c r="G30" s="43">
@@ -5940,7 +5964,7 @@
         <v>0.05</v>
       </c>
       <c r="I30" s="45">
-        <f t="shared" ref="I30:I31" si="22">IF(OR(F30=0,E30=0)," - ",NETWORKDAYS(E30,F30))</f>
+        <f t="shared" ref="I30:I31" si="23">IF(OR(F30=0,E30=0)," - ",NETWORKDAYS(E30,F30))</f>
         <v>1</v>
       </c>
       <c r="J30" s="46"/>
@@ -6043,9 +6067,9 @@
       <c r="DC30" s="37"/>
       <c r="DD30" s="37"/>
     </row>
-    <row r="31" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.4.2</v>
       </c>
       <c r="B31" s="47" t="s">
@@ -6056,7 +6080,7 @@
         <v>45084</v>
       </c>
       <c r="F31" s="42">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>45084</v>
       </c>
       <c r="G31" s="43">
@@ -6066,7 +6090,7 @@
         <v>0.05</v>
       </c>
       <c r="I31" s="45">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="J31" s="46"/>
@@ -6169,9 +6193,9 @@
       <c r="DC31" s="37"/>
       <c r="DD31" s="37"/>
     </row>
-    <row r="32" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.5</v>
       </c>
       <c r="B32" s="38" t="s">
@@ -6182,7 +6206,7 @@
         <v>45084</v>
       </c>
       <c r="F32" s="42">
-        <f t="shared" ref="F32:F34" si="23">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
+        <f t="shared" ref="F32:F34" si="24">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
         <v>45086</v>
       </c>
       <c r="G32" s="43">
@@ -6192,7 +6216,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="45">
-        <f t="shared" ref="I32:I34" si="24">IF(OR(F32=0,E32=0)," - ",NETWORKDAYS(E32,F32))</f>
+        <f t="shared" ref="I32:I34" si="25">IF(OR(F32=0,E32=0)," - ",NETWORKDAYS(E32,F32))</f>
         <v>3</v>
       </c>
       <c r="J32" s="46"/>
@@ -6295,9 +6319,9 @@
       <c r="DC32" s="37"/>
       <c r="DD32" s="37"/>
     </row>
-    <row r="33" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5.1</v>
       </c>
       <c r="B33" s="47" t="s">
@@ -6308,7 +6332,7 @@
         <v>45084</v>
       </c>
       <c r="F33" s="42">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>45084</v>
       </c>
       <c r="G33" s="43">
@@ -6318,7 +6342,7 @@
         <v>0.05</v>
       </c>
       <c r="I33" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="J33" s="46"/>
@@ -6421,9 +6445,9 @@
       <c r="DC33" s="37"/>
       <c r="DD33" s="37"/>
     </row>
-    <row r="34" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.5.2</v>
       </c>
       <c r="B34" s="47" t="s">
@@ -6434,7 +6458,7 @@
         <v>45084</v>
       </c>
       <c r="F34" s="42">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>45084</v>
       </c>
       <c r="G34" s="43">
@@ -6444,7 +6468,7 @@
         <v>0.05</v>
       </c>
       <c r="I34" s="45">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="J34" s="46"/>
@@ -6547,9 +6571,9 @@
       <c r="DC34" s="37"/>
       <c r="DD34" s="37"/>
     </row>
-    <row r="35" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="37" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.6</v>
       </c>
       <c r="B35" s="38" t="s">
@@ -6560,7 +6584,7 @@
         <v>45084</v>
       </c>
       <c r="F35" s="42">
-        <f t="shared" ref="F35:F39" si="25">IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
+        <f t="shared" ref="F35:F39" si="26">IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
         <v>45086</v>
       </c>
       <c r="G35" s="43">
@@ -6570,7 +6594,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="45">
-        <f t="shared" ref="I35:I39" si="26">IF(OR(F35=0,E35=0)," - ",NETWORKDAYS(E35,F35))</f>
+        <f t="shared" ref="I35:I39" si="27">IF(OR(F35=0,E35=0)," - ",NETWORKDAYS(E35,F35))</f>
         <v>3</v>
       </c>
       <c r="J35" s="46"/>
@@ -6673,9 +6697,9 @@
       <c r="DC35" s="37"/>
       <c r="DD35" s="37"/>
     </row>
-    <row r="36" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.6.1</v>
       </c>
       <c r="B36" s="47" t="s">
@@ -6686,7 +6710,7 @@
         <v>45084</v>
       </c>
       <c r="F36" s="42">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>45084</v>
       </c>
       <c r="G36" s="43">
@@ -6696,7 +6720,7 @@
         <v>0.05</v>
       </c>
       <c r="I36" s="45">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="J36" s="46"/>
@@ -6799,9 +6823,9 @@
       <c r="DC36" s="37"/>
       <c r="DD36" s="37"/>
     </row>
-    <row r="37" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.7</v>
       </c>
       <c r="B37" s="38" t="s">
@@ -6812,7 +6836,7 @@
         <v>45084</v>
       </c>
       <c r="F37" s="42">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>45086</v>
       </c>
       <c r="G37" s="43">
@@ -6822,7 +6846,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="45">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>3</v>
       </c>
       <c r="J37" s="46"/>
@@ -6925,9 +6949,9 @@
       <c r="DC37" s="37"/>
       <c r="DD37" s="37"/>
     </row>
-    <row r="38" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.7.1</v>
       </c>
       <c r="B38" s="47" t="s">
@@ -6938,7 +6962,7 @@
         <v>45084</v>
       </c>
       <c r="F38" s="42">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>45084</v>
       </c>
       <c r="G38" s="43">
@@ -6948,7 +6972,7 @@
         <v>0.05</v>
       </c>
       <c r="I38" s="45">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="J38" s="46"/>
@@ -7051,9 +7075,9 @@
       <c r="DC38" s="37"/>
       <c r="DD38" s="37"/>
     </row>
-    <row r="39" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.7.2</v>
       </c>
       <c r="B39" s="47" t="s">
@@ -7064,7 +7088,7 @@
         <v>45084</v>
       </c>
       <c r="F39" s="42">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>45084</v>
       </c>
       <c r="G39" s="43">
@@ -7074,7 +7098,7 @@
         <v>0.05</v>
       </c>
       <c r="I39" s="45">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="J39" s="46"/>
@@ -7177,7 +7201,7 @@
       <c r="DC39" s="37"/>
       <c r="DD39" s="37"/>
     </row>
-    <row r="40" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A40" s="37"/>
       <c r="B40" s="47"/>
       <c r="D40" s="40"/>
@@ -7286,7 +7310,7 @@
       <c r="DC40" s="37"/>
       <c r="DD40" s="37"/>
     </row>
-    <row r="41" spans="1:108" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:108" s="36" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -7297,13 +7321,13 @@
       <c r="D41" s="50"/>
       <c r="E41" s="51"/>
       <c r="F41" s="51" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G41" s="52"/>
       <c r="H41" s="53"/>
       <c r="I41" s="54" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J41" s="55"/>
@@ -7406,7 +7430,7 @@
       <c r="DC41" s="56"/>
       <c r="DD41" s="56"/>
     </row>
-    <row r="42" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -7419,7 +7443,7 @@
         <v>45121</v>
       </c>
       <c r="F42" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45150</v>
       </c>
       <c r="G42" s="43">
@@ -7429,7 +7453,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="J42" s="46"/>
@@ -7532,7 +7556,7 @@
       <c r="DC42" s="37"/>
       <c r="DD42" s="37"/>
     </row>
-    <row r="43" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A43" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.2</v>
@@ -7545,7 +7569,7 @@
         <v>45121</v>
       </c>
       <c r="F43" s="42">
-        <f t="shared" ref="F43" si="27">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
+        <f t="shared" ref="F43" si="28">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
         <v>45150</v>
       </c>
       <c r="G43" s="43">
@@ -7555,7 +7579,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="45">
-        <f t="shared" ref="I43" si="28">IF(OR(F43=0,E43=0)," - ",NETWORKDAYS(E43,F43))</f>
+        <f t="shared" ref="I43" si="29">IF(OR(F43=0,E43=0)," - ",NETWORKDAYS(E43,F43))</f>
         <v>21</v>
       </c>
       <c r="J43" s="46"/>
@@ -7658,7 +7682,7 @@
       <c r="DC43" s="37"/>
       <c r="DD43" s="37"/>
     </row>
-    <row r="44" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A44" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.3</v>
@@ -7671,7 +7695,7 @@
         <v>45121</v>
       </c>
       <c r="F44" s="42">
-        <f t="shared" ref="F44" si="29">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
+        <f t="shared" ref="F44" si="30">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
         <v>45150</v>
       </c>
       <c r="G44" s="43">
@@ -7681,7 +7705,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="45">
-        <f t="shared" ref="I44" si="30">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
+        <f t="shared" ref="I44" si="31">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
         <v>21</v>
       </c>
       <c r="J44" s="46"/>
@@ -7784,7 +7808,7 @@
       <c r="DC44" s="37"/>
       <c r="DD44" s="37"/>
     </row>
-    <row r="45" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:108" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A45" s="37"/>
       <c r="B45" s="38" t="s">
         <v>149</v>
@@ -7895,7 +7919,7 @@
       <c r="DC45" s="37"/>
       <c r="DD45" s="37"/>
     </row>
-    <row r="46" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>0.1</v>
@@ -7908,7 +7932,7 @@
         <v>45121</v>
       </c>
       <c r="F46" s="42">
-        <f t="shared" ref="F46" si="31">IF(ISBLANK(E46)," - ",IF(G46=0,E46,E46+G46-1))</f>
+        <f t="shared" ref="F46" si="32">IF(ISBLANK(E46)," - ",IF(G46=0,E46,E46+G46-1))</f>
         <v>45150</v>
       </c>
       <c r="G46" s="43">
@@ -7918,7 +7942,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="45">
-        <f t="shared" ref="I46" si="32">IF(OR(F46=0,E46=0)," - ",NETWORKDAYS(E46,F46))</f>
+        <f t="shared" ref="I46" si="33">IF(OR(F46=0,E46=0)," - ",NETWORKDAYS(E46,F46))</f>
         <v>21</v>
       </c>
       <c r="J46" s="46"/>
@@ -8021,7 +8045,7 @@
       <c r="DC46" s="37"/>
       <c r="DD46" s="37"/>
     </row>
-    <row r="47" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A47" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>0.1.1</v>
@@ -8034,7 +8058,7 @@
         <v>45121</v>
       </c>
       <c r="F47" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45135</v>
       </c>
       <c r="G47" s="43">
@@ -8044,7 +8068,7 @@
         <v>0.05</v>
       </c>
       <c r="I47" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="J47" s="46"/>
@@ -8147,7 +8171,7 @@
       <c r="DC47" s="37"/>
       <c r="DD47" s="37"/>
     </row>
-    <row r="48" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>0.1.2</v>
@@ -8160,7 +8184,7 @@
         <v>45139</v>
       </c>
       <c r="F48" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45153</v>
       </c>
       <c r="G48" s="43">
@@ -8170,7 +8194,7 @@
         <v>0.05</v>
       </c>
       <c r="I48" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="J48" s="46"/>
@@ -8273,7 +8297,7 @@
       <c r="DC48" s="37"/>
       <c r="DD48" s="37"/>
     </row>
-    <row r="49" spans="1:108" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:108" s="36" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -8284,13 +8308,13 @@
       <c r="D49" s="50"/>
       <c r="E49" s="51"/>
       <c r="F49" s="51" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G49" s="52"/>
       <c r="H49" s="53"/>
       <c r="I49" s="54" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J49" s="55"/>
@@ -8393,7 +8417,7 @@
       <c r="DC49" s="56"/>
       <c r="DD49" s="56"/>
     </row>
-    <row r="50" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A50" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -8406,7 +8430,7 @@
         <v>45154</v>
       </c>
       <c r="F50" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45168</v>
       </c>
       <c r="G50" s="43">
@@ -8416,7 +8440,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="J50" s="46"/>
@@ -8519,7 +8543,7 @@
       <c r="DC50" s="37"/>
       <c r="DD50" s="37"/>
     </row>
-    <row r="51" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A51" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.2</v>
@@ -8532,7 +8556,7 @@
         <v>45154</v>
       </c>
       <c r="F51" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45154</v>
       </c>
       <c r="G51" s="43">
@@ -8542,7 +8566,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J51" s="46"/>
@@ -8645,7 +8669,7 @@
       <c r="DC51" s="37"/>
       <c r="DD51" s="37"/>
     </row>
-    <row r="52" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.3</v>
@@ -8658,7 +8682,7 @@
         <v>45155</v>
       </c>
       <c r="F52" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45155</v>
       </c>
       <c r="G52" s="43">
@@ -8668,7 +8692,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J52" s="46"/>
@@ -8771,7 +8795,7 @@
       <c r="DC52" s="37"/>
       <c r="DD52" s="37"/>
     </row>
-    <row r="53" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A53" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.4</v>
@@ -8784,7 +8808,7 @@
         <v>45156</v>
       </c>
       <c r="F53" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45156</v>
       </c>
       <c r="G53" s="43">
@@ -8794,7 +8818,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J53" s="46"/>
@@ -8897,7 +8921,7 @@
       <c r="DC53" s="37"/>
       <c r="DD53" s="37"/>
     </row>
-    <row r="54" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.5</v>
@@ -8910,7 +8934,7 @@
         <v>45156</v>
       </c>
       <c r="F54" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45156</v>
       </c>
       <c r="G54" s="43">
@@ -8920,7 +8944,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J54" s="46"/>
@@ -9023,7 +9047,7 @@
       <c r="DC54" s="37"/>
       <c r="DD54" s="37"/>
     </row>
-    <row r="55" spans="1:108" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:108" s="36" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -9143,9 +9167,9 @@
       <c r="DC55" s="56"/>
       <c r="DD55" s="56"/>
     </row>
-    <row r="56" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:108" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A56" s="37" t="str">
-        <f t="shared" ref="A56" si="33">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A56" si="34">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B56" s="38" t="s">
@@ -9269,7 +9293,7 @@
       <c r="DC56" s="37"/>
       <c r="DD56" s="37"/>
     </row>
-    <row r="57" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A57" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.1.1</v>
@@ -9395,7 +9419,7 @@
       <c r="DC57" s="37"/>
       <c r="DD57" s="37"/>
     </row>
-    <row r="58" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A58" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.1.2</v>
@@ -9521,7 +9545,7 @@
       <c r="DC58" s="37"/>
       <c r="DD58" s="37"/>
     </row>
-    <row r="59" spans="1:108" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:108" s="39" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A59" s="37" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.1.3</v>
@@ -9649,12 +9673,15 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
     <mergeCell ref="CC4:CI4"/>
     <mergeCell ref="CJ4:CP4"/>
     <mergeCell ref="CQ4:CW4"/>
@@ -9671,15 +9698,12 @@
     <mergeCell ref="BH4:BN4"/>
     <mergeCell ref="BO4:BU4"/>
     <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="Y4:AE4"/>
   </mergeCells>
   <conditionalFormatting sqref="H8:H59">
     <cfRule type="dataBar" priority="1">
@@ -9714,7 +9738,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="H4" xr:uid="{E557819C-C82B-4BB1-B97B-E340AF4044FD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="H4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9730,15 +9754,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>99060</xdr:colOff>
+                    <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>121920</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>28</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>160020</xdr:rowOff>
+                    <xdr:rowOff>161925</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9773,21 +9797,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C220D389-2787-4D2C-9681-71929385216C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>34</v>
       </c>
@@ -9798,7 +9822,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="58">
         <v>1</v>
       </c>
@@ -9809,7 +9833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -9820,7 +9844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -9831,7 +9855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="58">
         <v>4</v>
       </c>
@@ -9848,188 +9872,188 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3030B70-32BB-45ED-B6AC-B5CC9DCEC36C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="106.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="71" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="70"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="71"/>
-      <c r="D9" s="72" t="s">
+      <c r="D8" s="61"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="62"/>
+      <c r="D9" s="63" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C10" s="70" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="70"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C11" s="70"/>
-      <c r="D11" s="72" t="s">
+      <c r="D10" s="61"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="61"/>
+      <c r="D11" s="63" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C12" s="71"/>
-      <c r="D12" s="70"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="62"/>
+      <c r="D12" s="61"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="70"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C14" s="71" t="s">
+      <c r="C13" s="62"/>
+      <c r="D13" s="61"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="70"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="61"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="70"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="62"/>
+      <c r="D15" s="61"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="70"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" s="62"/>
+      <c r="D16" s="61"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="70"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C18" s="71"/>
-      <c r="D18" s="70"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="62"/>
+      <c r="D17" s="61"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="62"/>
+      <c r="D18" s="61"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -10041,337 +10065,387 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0964A2-FC74-476E-A2C3-9AB491366E76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A68"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-    </row>
-    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A3" s="73" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="60"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A4" s="73" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="73" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="64" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="73" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="64" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" s="73" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A9" s="73" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="64" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="73" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="64" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="69" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
-    </row>
-    <row r="13" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A13" s="73" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="60"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="64" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="73" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="64" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="64" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="73" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="64" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="73" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="64" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="73" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="64" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="73" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="64" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" s="73" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="64" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="73" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="64" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="73" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="73" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="64" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="73" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="64" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="73" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="64" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="73" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="64" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="69" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="60" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="69"/>
-    </row>
-    <row r="29" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="73" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="60"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="64" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="73" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="64" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="73" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="64" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="73" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="64" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="73" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="64" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A34" s="73" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="64" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="73" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="64" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="73" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="64" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="69" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="60" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="69"/>
-    </row>
-    <row r="39" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="73" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="60"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="64" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="73" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="64" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="73" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="64" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A42" s="73" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="64" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="73" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="64" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="73" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="64" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="69" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="60" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="69"/>
-    </row>
-    <row r="47" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A47" s="73" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="60"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="64" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" s="73" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="64" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="73" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="64" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" s="73" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="64" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="69" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="60" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="69"/>
-    </row>
-    <row r="54" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A54" s="73" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="60"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="64" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" s="73" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="64" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="73" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="64" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" s="73" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="64" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A58" s="73" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="64" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" s="73" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="64" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A60" s="69" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="60" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A61" s="69"/>
-    </row>
-    <row r="62" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A62" s="73" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="60"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="64" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" s="73" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="64" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A64" s="73" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="64" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A65" s="73" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="64" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="73" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="64" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A67" s="73" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="64" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="15" x14ac:dyDescent="0.3">
-      <c r="A68" s="73" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="64" t="s">
         <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>